<commit_message>
Update Uebersicht Elemente Baernreither-Edition_2023.xlsx
</commit_message>
<xml_diff>
--- a/docs/Uebersicht Elemente Baernreither-Edition_2023.xlsx
+++ b/docs/Uebersicht Elemente Baernreither-Edition_2023.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="137">
   <si>
     <t>Übersicht über die für Baernreither-Edition verwendeten Elemtente</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>to</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
@@ -851,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1550,10 +1553,14 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="6"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="1"/>
+      <c r="A64" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>

</xml_diff>